<commit_message>
Regen all with `make all`
</commit_message>
<xml_diff>
--- a/project/excel/definedterm_profile.xlsx
+++ b/project/excel/definedterm_profile.xlsx
@@ -428,7 +428,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>identifier</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -479,7 +479,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>identifier</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -530,7 +530,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>identifier</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -591,7 +591,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>identifier</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -647,7 +647,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>identifier</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">

</xml_diff>